<commit_message>
Fix max memory per Node
Should be set the max memory per node, it had a wrong formula to
be calculate.
</commit_message>
<xml_diff>
--- a/fair-scheduler/Memory Configuration Settings Tutorial.xlsx
+++ b/fair-scheduler/Memory Configuration Settings Tutorial.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="135">
   <si>
     <t>Plan to calculate autonomus elasticity with Fair Scheduler [6][7]</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>yarn.nodemanager.resource.memory-mb</t>
+  </si>
+  <si>
+    <t>* Calculate directly from E20 and E21</t>
   </si>
   <si>
     <t>yarn.scheduler.minimum-allocation-mb</t>
@@ -762,7 +765,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1313,6 +1316,9 @@
       <c r="G27" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="H27" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
@@ -1322,7 +1328,7 @@
         <v>50</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D28" s="12" t="n">
         <f aca="false">C21</f>
@@ -1347,32 +1353,35 @@
         <v>50</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D29" s="12" t="n">
-        <f aca="false">C20*C21</f>
-        <v>12</v>
+        <f aca="false">F29/1024</f>
+        <v>13.333984375</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="12" t="n">
-        <f aca="false">ROUND(D29*1024)</f>
-        <v>12288</v>
+        <f aca="false">E20*E21</f>
+        <v>13654</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="H29" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D30" s="12" t="n">
         <f aca="false">C21</f>
@@ -1391,13 +1400,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D31" s="12" t="n">
         <f aca="false">2*C21</f>
@@ -1416,13 +1425,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D32" s="12" t="n">
         <f aca="false">0.8*C21</f>
@@ -1441,13 +1450,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D33" s="12" t="n">
         <f aca="false">0.8*2*C21</f>
@@ -1466,13 +1475,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D34" s="12" t="n">
         <f aca="false">2*C21</f>
@@ -1491,13 +1500,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D35" s="12" t="n">
         <f aca="false">0.8*2*C21</f>
@@ -1516,25 +1525,25 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D36" s="12" t="n">
         <v>2.1</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F36" s="12" t="n">
         <v>2.1</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,7 +1556,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="0"/>
@@ -1555,7 +1564,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B40" s="23"/>
       <c r="C40" s="0"/>
@@ -1563,7 +1572,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="0"/>
@@ -1571,7 +1580,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="0"/>
@@ -1579,7 +1588,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="0"/>
@@ -1595,7 +1604,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="0"/>
@@ -1603,7 +1612,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="0"/>
@@ -1611,105 +1620,105 @@
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B48" s="25"/>
       <c r="C48" s="25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48" s="25"/>
     </row>
     <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B49" s="25"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B51" s="21"/>
     </row>
     <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B52" s="25"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1776,271 +1785,271 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update and improve Fair Scheduler Memory confs and Collectd metrics
Has been update the configuration of the Hadoop Memory fair scheduler,
also has been splited the process to monitoring the cluster to
scale up or down according to the workload of the cluster.
</commit_message>
<xml_diff>
--- a/fair-scheduler/Memory Configuration Settings Tutorial.xlsx
+++ b/fair-scheduler/Memory Configuration Settings Tutorial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="212" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="226" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Based upon memory" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
   <si>
     <t>Plan to calculate autonomus elasticity with Fair Scheduler [6][7]</t>
   </si>
@@ -78,7 +78,7 @@
     <t>Available RAM Worker</t>
   </si>
   <si>
-    <t>[13] “... 10-20% of RAM for Linux and its daemon services..”  “Example takes it into account”[2]</t>
+    <t>[13] “... 10-20% of RAM for Linux and its daemon services..”  “Example takes it into account”[2] To be exaxt this value has been taken from a deploy when the yarn shows through the GUI the “Total Memory” divide by #Worker nodes</t>
   </si>
   <si>
     <t>vCores</t>
@@ -174,9 +174,6 @@
     <t>yarn.nodemanager.resource.memory-mb</t>
   </si>
   <si>
-    <t>* Calculate directly from E20 and E21</t>
-  </si>
-  <si>
     <t>yarn.scheduler.minimum-allocation-mb</t>
   </si>
   <si>
@@ -306,115 +303,115 @@
     <t>[14] http://www.binarytides.com/linux-check-processor/</t>
   </si>
   <si>
-    <t>yarn.QueueMetrics: Queue=root, </t>
-  </si>
-  <si>
-    <t>yarn.QueueMetrics: Queue=root.panacea, </t>
-  </si>
-  <si>
-    <t>User=hadoop, </t>
-  </si>
-  <si>
-    <t>Context=yarn, </t>
-  </si>
-  <si>
-    <t>Hostname=Hop-ResourceMan, </t>
-  </si>
-  <si>
-    <t>running_0=0, </t>
-  </si>
-  <si>
-    <t>running_60=0, </t>
-  </si>
-  <si>
-    <t>running_300=0, </t>
-  </si>
-  <si>
-    <t>running_1440=0, </t>
-  </si>
-  <si>
-    <t>FairShareMB=0, </t>
-  </si>
-  <si>
-    <t>FairShareVCores=0, </t>
-  </si>
-  <si>
-    <t>SteadyFairShareMB=12288, </t>
-  </si>
-  <si>
-    <t>SteadyFairShareVCores=0, </t>
-  </si>
-  <si>
-    <t>MinShareMB=1024, </t>
-  </si>
-  <si>
-    <t>MinShareVCores=1, </t>
-  </si>
-  <si>
-    <t>MaxShareMB=24576, </t>
-  </si>
-  <si>
-    <t>MaxShareVCores=24, </t>
-  </si>
-  <si>
-    <t>AppsSubmitted=1, </t>
-  </si>
-  <si>
-    <t>AppsRunning=0, </t>
-  </si>
-  <si>
-    <t>AppsPending=0, </t>
-  </si>
-  <si>
-    <t>AppsCompleted=1, </t>
-  </si>
-  <si>
-    <t>AppsKilled=0, </t>
-  </si>
-  <si>
-    <t>AppsFailed=0, </t>
-  </si>
-  <si>
-    <t>AllocatedMB=0, </t>
-  </si>
-  <si>
-    <t>AllocatedVCores=0, </t>
-  </si>
-  <si>
-    <t>AllocatedContainers=0, </t>
-  </si>
-  <si>
-    <t>AggregateContainersAllocated=34, </t>
-  </si>
-  <si>
-    <t>AggregateContainersReleased=34, </t>
-  </si>
-  <si>
-    <t>AvailableMB=0, </t>
-  </si>
-  <si>
-    <t>AvailableVCores=0, </t>
-  </si>
-  <si>
-    <t>PendingMB=0, </t>
-  </si>
-  <si>
-    <t>PendingVCores=0, </t>
-  </si>
-  <si>
-    <t>PendingContainers=0, </t>
-  </si>
-  <si>
-    <t>ReservedMB=0, </t>
-  </si>
-  <si>
-    <t>ReservedVCores=0, </t>
-  </si>
-  <si>
-    <t>ReservedContainers=0, </t>
-  </si>
-  <si>
-    <t>ActiveUsers=0, </t>
+    <t>yarn.QueueMetrics: Queue=root,</t>
+  </si>
+  <si>
+    <t>yarn.QueueMetrics: Queue=root.panacea,</t>
+  </si>
+  <si>
+    <t>User=hadoop,</t>
+  </si>
+  <si>
+    <t>Context=yarn,</t>
+  </si>
+  <si>
+    <t>Hostname=Hop-ResourceMan,</t>
+  </si>
+  <si>
+    <t>running_0=0,</t>
+  </si>
+  <si>
+    <t>running_60=0,</t>
+  </si>
+  <si>
+    <t>running_300=0,</t>
+  </si>
+  <si>
+    <t>running_1440=0,</t>
+  </si>
+  <si>
+    <t>FairShareMB=0,</t>
+  </si>
+  <si>
+    <t>FairShareVCores=0,</t>
+  </si>
+  <si>
+    <t>SteadyFairShareMB=12288,</t>
+  </si>
+  <si>
+    <t>SteadyFairShareVCores=0,</t>
+  </si>
+  <si>
+    <t>MinShareMB=1024,</t>
+  </si>
+  <si>
+    <t>MinShareVCores=1,</t>
+  </si>
+  <si>
+    <t>MaxShareMB=24576,</t>
+  </si>
+  <si>
+    <t>MaxShareVCores=24,</t>
+  </si>
+  <si>
+    <t>AppsSubmitted=1,</t>
+  </si>
+  <si>
+    <t>AppsRunning=0,</t>
+  </si>
+  <si>
+    <t>AppsPending=0,</t>
+  </si>
+  <si>
+    <t>AppsCompleted=1,</t>
+  </si>
+  <si>
+    <t>AppsKilled=0,</t>
+  </si>
+  <si>
+    <t>AppsFailed=0,</t>
+  </si>
+  <si>
+    <t>AllocatedMB=0,</t>
+  </si>
+  <si>
+    <t>AllocatedVCores=0,</t>
+  </si>
+  <si>
+    <t>AllocatedContainers=0,</t>
+  </si>
+  <si>
+    <t>AggregateContainersAllocated=34,</t>
+  </si>
+  <si>
+    <t>AggregateContainersReleased=34,</t>
+  </si>
+  <si>
+    <t>AvailableMB=0,</t>
+  </si>
+  <si>
+    <t>AvailableVCores=0,</t>
+  </si>
+  <si>
+    <t>PendingMB=0,</t>
+  </si>
+  <si>
+    <t>PendingVCores=0,</t>
+  </si>
+  <si>
+    <t>PendingContainers=0,</t>
+  </si>
+  <si>
+    <t>ReservedMB=0,</t>
+  </si>
+  <si>
+    <t>ReservedVCores=0,</t>
+  </si>
+  <si>
+    <t>ReservedContainers=0,</t>
+  </si>
+  <si>
+    <t>ActiveUsers=0,</t>
   </si>
   <si>
     <t>ActiveUsers=0, Ç</t>
@@ -505,7 +502,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +519,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
         <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -572,7 +575,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -629,11 +632,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -765,7 +776,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -891,15 +902,15 @@
       <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12" t="n">
-        <v>1</v>
+      <c r="C7" s="14" t="n">
+        <v>4</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="12" t="n">
         <f aca="false">C7</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
@@ -965,16 +976,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="12" t="n">
-        <f aca="false">ROUND(C9*0.9)</f>
-        <v>14</v>
+        <v>13.33</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -1007,14 +1017,14 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
       <c r="H12" s="7" t="n">
         <v>256</v>
       </c>
@@ -1023,19 +1033,19 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15" t="n">
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="n">
         <f aca="false">C7*C5</f>
-        <v>3</v>
-      </c>
-      <c r="D13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
+      <c r="D13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="7" t="n">
@@ -1046,39 +1056,39 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15" t="n">
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="n">
         <f aca="false">C8*C5</f>
         <v>3</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15" t="n">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="n">
         <f aca="false">C10*C5</f>
-        <v>42</v>
-      </c>
-      <c r="D15" s="15" t="s">
+        <v>39.99</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="15" t="n">
+      <c r="E15" s="17" t="n">
         <f aca="false">C15*1024</f>
-        <v>43008</v>
-      </c>
-      <c r="F15" s="15" t="s">
+        <v>40949.76</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1157,7 +1167,7 @@
       <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="16" t="str">
+      <c r="C19" s="18" t="str">
         <f aca="false">IF(C10&lt;I17,"0.25",IF(AND(C10&gt;=I17,C10 &lt; I18),"0.5",IF(AND(C10&gt;=I18,C10 &lt; I19),"1","2")))</f>
         <v>1</v>
       </c>
@@ -1190,7 +1200,7 @@
       </c>
       <c r="C20" s="12" t="n">
         <f aca="false">MIN(2*C8,1.8*C7,(C10-C18)/C19)</f>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>40</v>
@@ -1219,24 +1229,24 @@
       </c>
       <c r="C21" s="12" t="n">
         <f aca="false">MAX(C19,(C10-C18)/C20)</f>
-        <v>6.66666666666667</v>
+        <v>5.665</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="12" t="n">
         <f aca="false">ROUND(C21*1024)</f>
-        <v>6827</v>
+        <v>5801</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
@@ -1296,50 +1306,47 @@
       <c r="A27" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="12" t="n">
-        <f aca="false">F27/1024</f>
-        <v>13.333984375</v>
+        <f aca="false">C20*C21</f>
+        <v>11.33</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="12" t="n">
-        <f aca="false">E20*E21</f>
-        <v>13654</v>
+        <f aca="false">D27*1024</f>
+        <v>11601.92</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="12" t="n">
         <f aca="false">C21</f>
-        <v>6.66666666666667</v>
+        <v>5.665</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="12" t="n">
-        <f aca="false">ROUND(D28*1024)</f>
-        <v>6827</v>
+        <f aca="false">D28*1024</f>
+        <v>5800.96</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>18</v>
@@ -1349,50 +1356,47 @@
       <c r="A29" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29" s="12" t="n">
-        <f aca="false">F29/1024</f>
-        <v>13.333984375</v>
+        <f aca="false">C20*C21</f>
+        <v>11.33</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="12" t="n">
-        <f aca="false">E20*E21</f>
-        <v>13654</v>
+        <f aca="false">D29*1024</f>
+        <v>11601.92</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="D30" s="12" t="n">
         <f aca="false">C21</f>
-        <v>6.66666666666667</v>
+        <v>5.665</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="12" t="n">
-        <f aca="false">ROUND(D30*1024)</f>
-        <v>6827</v>
+        <f aca="false">D30*1024</f>
+        <v>5800.96</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>18</v>
@@ -1400,24 +1404,24 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="D31" s="12" t="n">
         <f aca="false">2*C21</f>
-        <v>13.3333333333333</v>
+        <v>11.33</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="12" t="n">
-        <f aca="false">ROUND(D31*1024)</f>
-        <v>13653</v>
+        <f aca="false">D31*1024</f>
+        <v>11601.92</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>18</v>
@@ -1425,24 +1429,24 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>56</v>
-      </c>
       <c r="C32" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D32" s="12" t="n">
         <f aca="false">0.8*C21</f>
-        <v>5.33333333333333</v>
+        <v>4.532</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F32" s="12" t="n">
-        <f aca="false">ROUND(D32*1024)</f>
-        <v>5461</v>
+        <f aca="false">D32*1024</f>
+        <v>4640.768</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>18</v>
@@ -1450,24 +1454,24 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>56</v>
-      </c>
       <c r="C33" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="12" t="n">
         <f aca="false">0.8*2*C21</f>
-        <v>10.6666666666667</v>
+        <v>9.064</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="12" t="n">
-        <f aca="false">ROUND(D33*1024)</f>
-        <v>10923</v>
+        <f aca="false">D33*1024</f>
+        <v>9281.536</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>18</v>
@@ -1475,24 +1479,24 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="D34" s="12" t="n">
         <f aca="false">2*C21</f>
-        <v>13.3333333333333</v>
+        <v>11.33</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F34" s="12" t="n">
-        <f aca="false">ROUND(D34*1024)</f>
-        <v>13653</v>
+        <f aca="false">D34*1024</f>
+        <v>11601.92</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>18</v>
@@ -1500,24 +1504,24 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>63</v>
-      </c>
       <c r="C35" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" s="12" t="n">
         <f aca="false">0.8*2*C21</f>
-        <v>10.6666666666667</v>
+        <v>9.064</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F35" s="12" t="n">
-        <f aca="false">ROUND(D35*1024)</f>
-        <v>10923</v>
+        <f aca="false">D35*1024</f>
+        <v>9281.536</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>18</v>
@@ -1525,25 +1529,25 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="D36" s="12" t="n">
         <v>2.1</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F36" s="12" t="n">
         <v>2.1</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,42 +1559,42 @@
       <c r="D38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="24"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="0"/>
-      <c r="D39" s="22"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="23"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="0"/>
       <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="23"/>
+      <c r="A41" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="25"/>
       <c r="C41" s="0"/>
       <c r="D41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="23"/>
+      <c r="A42" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="25"/>
       <c r="C42" s="0"/>
       <c r="D42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="23"/>
+      <c r="A43" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="25"/>
       <c r="C43" s="0"/>
       <c r="D43" s="0"/>
     </row>
@@ -1603,122 +1607,122 @@
       <c r="D45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="21"/>
+      <c r="A46" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="23"/>
       <c r="C46" s="0"/>
       <c r="D46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="24"/>
+      <c r="A47" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="26"/>
       <c r="C47" s="0"/>
       <c r="D47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25" t="s">
+      <c r="D48" s="27"/>
+    </row>
+    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="25"/>
-    </row>
-    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="25" t="s">
+      <c r="B49" s="27"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="25"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="21" t="s">
+      <c r="B51" s="23"/>
+    </row>
+    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="21"/>
-    </row>
-    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="25" t="s">
+      <c r="B52" s="27"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="25"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="26" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="27" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="27" t="s">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="27" t="s">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="27" t="s">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="27" t="s">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="27" t="s">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="27" t="s">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="27" t="s">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="27" t="s">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="27" t="s">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="29" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="27" t="s">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="29" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="27" t="s">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="27" t="s">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="29" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="27" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1784,272 +1788,272 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>96</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>